<commit_message>
Added Readme file, cleaned up the code
</commit_message>
<xml_diff>
--- a/fw_rules_test.xlsx
+++ b/fw_rules_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D528C690-3206-487C-A822-774C06EBB518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD0BF4-C99C-48E4-9BDB-2DC8EE3A9B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Feedback" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$L$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$K$8</definedName>
     <definedName name="BulkData">'Dropdown Fields'!#REF!</definedName>
     <definedName name="Customer">'Dropdown Fields'!#REF!</definedName>
     <definedName name="DestinationProtocol">'Dropdown Fields'!#REF!</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="214">
   <si>
     <t>Source Network</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Insert - &gt; Table</t>
   </si>
   <si>
-    <t>Enter formula as =INDIRECT("TableName[Column1]")</t>
-  </si>
-  <si>
     <t>How to add a New Dropdown Column</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Digital Media Content</t>
   </si>
   <si>
-    <t>Comment:</t>
-  </si>
-  <si>
     <t>Source Zone</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>dmz-internal</t>
   </si>
   <si>
-    <t>DMZ1 - semi-trusted - LB services - private adderees</t>
-  </si>
-  <si>
     <t>Device Mgmt</t>
   </si>
   <si>
@@ -174,12 +165,6 @@
     <t>Delete</t>
   </si>
   <si>
-    <t>Source Port</t>
-  </si>
-  <si>
-    <t>Rule Name</t>
-  </si>
-  <si>
     <t>10.64.0.0/16, 10.5.0.0/28</t>
   </si>
   <si>
@@ -189,9 +174,6 @@
     <t>servers1</t>
   </si>
   <si>
-    <t>10.78.0.0/24</t>
-  </si>
-  <si>
     <t>internet-untrust</t>
   </si>
   <si>
@@ -204,51 +186,9 @@
     <t>88.3.98.2/32</t>
   </si>
   <si>
-    <t>globtftp01</t>
-  </si>
-  <si>
-    <t>esbu-172-supernet</t>
-  </si>
-  <si>
-    <t>172.16.0.0/12</t>
-  </si>
-  <si>
-    <t>azure-aus-jumphost</t>
-  </si>
-  <si>
-    <t>10.248.58.128/26</t>
-  </si>
-  <si>
-    <t>azure-aue-jumphost</t>
-  </si>
-  <si>
-    <t>10.248.56.128/26</t>
-  </si>
-  <si>
-    <t>azure-aus-aue-supernet</t>
-  </si>
-  <si>
     <t>10.248.56.0/21</t>
   </si>
   <si>
-    <t>portpuppet01</t>
-  </si>
-  <si>
-    <t>globswsat01</t>
-  </si>
-  <si>
-    <t>172.16.40.72/32</t>
-  </si>
-  <si>
-    <t>portswsat01</t>
-  </si>
-  <si>
-    <t>172.21.40.72/32</t>
-  </si>
-  <si>
-    <t>azure-aus-spacewalk</t>
-  </si>
-  <si>
     <t>azure-aue-spacewalk</t>
   </si>
   <si>
@@ -258,39 +198,12 @@
     <t>10.248.56.192/26</t>
   </si>
   <si>
-    <t>azure-aus-ad-group</t>
-  </si>
-  <si>
     <t>10.248.58.192/26</t>
   </si>
   <si>
-    <t>globrhsat01</t>
-  </si>
-  <si>
-    <t>172.16.40.226/32</t>
-  </si>
-  <si>
-    <t>portrhsat01</t>
-  </si>
-  <si>
     <t>172.21.40.226/32</t>
   </si>
   <si>
-    <t>globdcs01</t>
-  </si>
-  <si>
-    <t>172.17.6.20/32</t>
-  </si>
-  <si>
-    <t>globdcs02</t>
-  </si>
-  <si>
-    <t>172.17.6.21/32</t>
-  </si>
-  <si>
-    <t>azure-aus-redhat01</t>
-  </si>
-  <si>
     <t>10.248.59.21/32</t>
   </si>
   <si>
@@ -300,27 +213,15 @@
     <t>10.248.57.21/32</t>
   </si>
   <si>
-    <t>portdcs02</t>
-  </si>
-  <si>
     <t>172.21.6.21/32</t>
   </si>
   <si>
-    <t>portdcs01</t>
-  </si>
-  <si>
     <t>172.21.6.20/32</t>
   </si>
   <si>
-    <t>portrepo01</t>
-  </si>
-  <si>
     <t>172.21.40.21/32</t>
   </si>
   <si>
-    <t>globansible01</t>
-  </si>
-  <si>
     <t>azure-host-10.248.56.200</t>
   </si>
   <si>
@@ -333,12 +234,6 @@
     <t>10.248.56.201/32</t>
   </si>
   <si>
-    <t>globca01</t>
-  </si>
-  <si>
-    <t>172.17.6.40/32</t>
-  </si>
-  <si>
     <t>aueats01</t>
   </si>
   <si>
@@ -351,198 +246,21 @@
     <t>10.248.56.151/32</t>
   </si>
   <si>
-    <t>ausets01</t>
-  </si>
-  <si>
     <t>10.248.58.150/32</t>
   </si>
   <si>
-    <t>ausets02</t>
-  </si>
-  <si>
     <t>10.248.58.151/32</t>
   </si>
   <si>
-    <t>globkms01</t>
-  </si>
-  <si>
-    <t>172.16.40.10/32</t>
-  </si>
-  <si>
-    <t>aueagraylog01</t>
-  </si>
-  <si>
-    <t>10.248.57.30/32</t>
-  </si>
-  <si>
-    <t>aueagraylog02</t>
-  </si>
-  <si>
-    <t>10.248.57.31/32</t>
-  </si>
-  <si>
-    <t>aueagraylog03</t>
-  </si>
-  <si>
-    <t>10.248.57.32/32</t>
-  </si>
-  <si>
-    <t>aueagraylog04</t>
-  </si>
-  <si>
-    <t>10.248.57.33/32</t>
-  </si>
-  <si>
-    <t>globkafka01</t>
-  </si>
-  <si>
-    <t>172.17.7.239/32</t>
-  </si>
-  <si>
-    <t>globkafka02</t>
-  </si>
-  <si>
-    <t>172.17.7.244/32</t>
-  </si>
-  <si>
-    <t>globkafka03</t>
-  </si>
-  <si>
-    <t>172.17.7.247/32</t>
-  </si>
-  <si>
-    <t>globkafka04</t>
-  </si>
-  <si>
-    <t>172.17.7.123/32</t>
-  </si>
-  <si>
-    <t>globkafka05</t>
-  </si>
-  <si>
-    <t>172.17.7.126/32</t>
-  </si>
-  <si>
-    <t>globkafka06</t>
-  </si>
-  <si>
-    <t>172.17.7.131/32</t>
-  </si>
-  <si>
-    <t>globgraylog11</t>
-  </si>
-  <si>
-    <t>172.17.7.9/32</t>
-  </si>
-  <si>
-    <t>globgraylog12</t>
-  </si>
-  <si>
-    <t>172.17.7.17/32</t>
-  </si>
-  <si>
-    <t>globgraylog13</t>
-  </si>
-  <si>
-    <t>172.17.7.22/32</t>
-  </si>
-  <si>
-    <t>globgraylog14</t>
-  </si>
-  <si>
-    <t>172.17.7.30/32</t>
-  </si>
-  <si>
-    <t>globgraylog15</t>
-  </si>
-  <si>
-    <t>172.17.7.32/32</t>
-  </si>
-  <si>
-    <t>globgraylog16</t>
-  </si>
-  <si>
-    <t>172.17.7.39/32</t>
-  </si>
-  <si>
-    <t>globgraylog17</t>
-  </si>
-  <si>
-    <t>172.17.7.44/32</t>
-  </si>
-  <si>
-    <t>globgraylog18</t>
-  </si>
-  <si>
-    <t>172.17.7.47/32</t>
-  </si>
-  <si>
-    <t>aueafrmnprxy01</t>
-  </si>
-  <si>
-    <t>10.248.57.50/32</t>
-  </si>
-  <si>
-    <t>globforeman01</t>
-  </si>
-  <si>
-    <t>172.17.7.138/32</t>
-  </si>
-  <si>
-    <t>globforeman02</t>
-  </si>
-  <si>
-    <t>172.17.7.129/32</t>
-  </si>
-  <si>
-    <t>aueapuppet01</t>
-  </si>
-  <si>
-    <t>ausepuppet01</t>
-  </si>
-  <si>
-    <t>10.248.59.50/32</t>
-  </si>
-  <si>
-    <t>globgit01</t>
-  </si>
-  <si>
-    <t>172.16.40.19/32</t>
-  </si>
-  <si>
-    <t>cbus-aapt-wan</t>
-  </si>
-  <si>
-    <t>172.22.0.0/24</t>
-  </si>
-  <si>
-    <t>cbus-aapt-tloc-172.23.0.0/24</t>
-  </si>
-  <si>
-    <t>172.23.0.0/24</t>
-  </si>
-  <si>
-    <t>globdwannetutil02</t>
-  </si>
-  <si>
-    <t>118.127.84.2/32</t>
-  </si>
-  <si>
     <t>Network</t>
   </si>
   <si>
-    <t>ESBU TFTP</t>
-  </si>
-  <si>
     <t>Azure Mgmt Hosts Net 1</t>
   </si>
   <si>
     <t>Azure Mgmt Hosts Net 2</t>
   </si>
   <si>
-    <t>globansible01, portpuppet01</t>
-  </si>
-  <si>
     <t>InterAct application Client to Server</t>
   </si>
   <si>
@@ -555,9 +273,6 @@
     <t>Test servers</t>
   </si>
   <si>
-    <t>azure-aus-redhat01, 10.1.2.0/24, aueafrmnprxy01</t>
-  </si>
-  <si>
     <t>Management FTP Infra Services</t>
   </si>
   <si>
@@ -573,9 +288,6 @@
     <t>automatic application to FWs - Jenkins/Ansible</t>
   </si>
   <si>
-    <t>any zone - create global rule</t>
-  </si>
-  <si>
     <t>dashes instead of _</t>
   </si>
   <si>
@@ -585,9 +297,6 @@
     <t>rules order - check</t>
   </si>
   <si>
-    <t>port ranges and list</t>
-  </si>
-  <si>
     <t>tcp</t>
   </si>
   <si>
@@ -597,18 +306,6 @@
     <t>Port</t>
   </si>
   <si>
-    <t>globansible01.esbu.local</t>
-  </si>
-  <si>
-    <t>globtftp01.esbu.local</t>
-  </si>
-  <si>
-    <t>portpuppet01.esbu.local</t>
-  </si>
-  <si>
-    <t>azure-serv-aus1.azure.net</t>
-  </si>
-  <si>
     <t>azure-serv-aue1.azure.net</t>
   </si>
   <si>
@@ -666,9 +363,6 @@
     <t>review process ?</t>
   </si>
   <si>
-    <t>globansible01, azure-host-10.248.56.200</t>
-  </si>
-  <si>
     <t>application-objects - groups , protocol - app-group</t>
   </si>
   <si>
@@ -865,6 +559,135 @@
   </si>
   <si>
     <t>aueats01, aueats02, 192.168.200.0/27</t>
+  </si>
+  <si>
+    <t>ndctftp01</t>
+  </si>
+  <si>
+    <t>ndcswsat01</t>
+  </si>
+  <si>
+    <t>ndcrhsat01</t>
+  </si>
+  <si>
+    <t>ndcdcs01</t>
+  </si>
+  <si>
+    <t>ndcdcs02</t>
+  </si>
+  <si>
+    <t>ndcansible01</t>
+  </si>
+  <si>
+    <t>ndcca01</t>
+  </si>
+  <si>
+    <t>ndckms01</t>
+  </si>
+  <si>
+    <t>any zone - create ndcal rule</t>
+  </si>
+  <si>
+    <t>172.23.6.20/32</t>
+  </si>
+  <si>
+    <t>172.23.6.21/32</t>
+  </si>
+  <si>
+    <t>172.23.6.40/32</t>
+  </si>
+  <si>
+    <t>ndcansible01, mdcpuppet01</t>
+  </si>
+  <si>
+    <t>mdcpuppet01</t>
+  </si>
+  <si>
+    <t>mdcswsat01</t>
+  </si>
+  <si>
+    <t>mdcrhsat01</t>
+  </si>
+  <si>
+    <t>mdcdcs02</t>
+  </si>
+  <si>
+    <t>mdcdcs01</t>
+  </si>
+  <si>
+    <t>mdcrepo01</t>
+  </si>
+  <si>
+    <t>mdc ranges and list</t>
+  </si>
+  <si>
+    <t>azure-rg-aue-supernet</t>
+  </si>
+  <si>
+    <t>azure-rg-spacewalk</t>
+  </si>
+  <si>
+    <t>azure-serv-rg1.azure.net</t>
+  </si>
+  <si>
+    <t>azure-rg-ad-group</t>
+  </si>
+  <si>
+    <t>azure-rg-redhat01</t>
+  </si>
+  <si>
+    <t>rgets01</t>
+  </si>
+  <si>
+    <t>rgets02</t>
+  </si>
+  <si>
+    <t>ndctftp01.mgmt.local</t>
+  </si>
+  <si>
+    <t>mgmt TFTP</t>
+  </si>
+  <si>
+    <t>mdcpuppet01.mgmt.local</t>
+  </si>
+  <si>
+    <t>ndcansible01.mgmt.local</t>
+  </si>
+  <si>
+    <t>172.20.72/32</t>
+  </si>
+  <si>
+    <t>172.24.40.72/32</t>
+  </si>
+  <si>
+    <t>172.20.226/32</t>
+  </si>
+  <si>
+    <t>172.26.10/32</t>
+  </si>
+  <si>
+    <t>Flow Name</t>
+  </si>
+  <si>
+    <t>10.248.158.128/26</t>
+  </si>
+  <si>
+    <t>10.248.156.128/26</t>
+  </si>
+  <si>
+    <t>azure-rg-jumphosts</t>
+  </si>
+  <si>
+    <t>azure-aue-jumphosts</t>
+  </si>
+  <si>
+    <t>mdcpuppet01, azure-rg-jumphosts</t>
+  </si>
+  <si>
+    <t>azure-aue-redhat01, 10.1.2.0/24</t>
+  </si>
+  <si>
+    <t>DMZ1 - semi-trusted - LB services - private addresses</t>
   </si>
 </sst>
 </file>
@@ -960,7 +783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1073,11 +896,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,6 +961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,7 +1183,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6988F3E5-D080-491E-8272-78CEDDC891B9}" name="Zone Name"/>
     <tableColumn id="3" xr3:uid="{6BAFF4A9-DA69-4132-96EE-4BCBAB6EC3C6}" name="Zone Set"/>
-    <tableColumn id="2" xr3:uid="{55518FE0-84A0-40A9-AAFF-A81147B7E0D2}" name="Comment:"/>
+    <tableColumn id="2" xr3:uid="{55518FE0-84A0-40A9-AAFF-A81147B7E0D2}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1707,337 +1544,312 @@
     <tabColor rgb="FF33CC33"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.88671875" style="8" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="11" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="47.77734375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="24.21875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="9" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="8"/>
+    <col min="3" max="3" width="21.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="47.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="9" style="8" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>206</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="10">
+        <v>8585</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="10">
+        <v>21</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="10">
         <v>22</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="10">
-        <v>8585</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="I8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="10">
-        <v>21</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="10">
-        <v>22</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="K2:K1048576">
+  <autoFilter ref="A1:K8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="J2:J1048576">
     <cfRule type="cellIs" dxfId="14" priority="4305" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2045,7 +1857,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L8">
+  <conditionalFormatting sqref="K3:K8">
     <cfRule type="cellIs" dxfId="12" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2053,12 +1865,12 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8 F3:F8">
+  <conditionalFormatting sqref="C3:C8 E3:E8">
     <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J8">
+  <conditionalFormatting sqref="I3:I8">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"deny"</formula>
     </cfRule>
@@ -2069,7 +1881,7 @@
       <formula>"permit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
+  <conditionalFormatting sqref="K2">
     <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2077,17 +1889,17 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
+  <conditionalFormatting sqref="E2">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"deny"</formula>
     </cfRule>
@@ -2099,19 +1911,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:J1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Boolean[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:D1048576 H9:H1048576 C2:C8" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G1048576 C9:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("DestProtoTable[Column1]")</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("ServiceTable[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8" xr:uid="{4D4FF7E8-FB77-4CF0-8941-3A2929C41218}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8" xr:uid="{4D4FF7E8-FB77-4CF0-8941-3A2929C41218}">
       <formula1>INDIRECT("DestProtoTable[Values]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L8" xr:uid="{2459F31B-84F4-40B3-8182-C99B6AF8BAD6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K8" xr:uid="{2459F31B-84F4-40B3-8182-C99B6AF8BAD6}">
       <formula1>INDIRECT("Boolean[Values]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2124,13 +1936,13 @@
           <x14:formula1>
             <xm:f>Zones!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8 D2:D8</xm:sqref>
+          <xm:sqref>E2:E8 C2:C8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD155D18-2081-4233-B9F7-E634676BB1FE}">
           <x14:formula1>
             <xm:f>'Dropdown Fields'!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J8</xm:sqref>
+          <xm:sqref>I2:I8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2143,10 +1955,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,10 +1970,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>166</v>
+        <v>72</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>160</v>
+        <v>68</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>3</v>
@@ -2169,467 +1981,243 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>163</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>129</v>
-      </c>
-      <c r="B43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>135</v>
-      </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>149</v>
-      </c>
-      <c r="B53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>150</v>
-      </c>
-      <c r="B54" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>154</v>
-      </c>
-      <c r="B56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>156</v>
-      </c>
-      <c r="B57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>158</v>
-      </c>
-      <c r="B58" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2645,149 +2233,151 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection sort="0" autoFilter="0"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2801,10 +2391,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2812,561 +2402,566 @@
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>253</v>
+        <v>151</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>153</v>
       </c>
       <c r="C2" s="24">
         <v>999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>153</v>
       </c>
       <c r="C3" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="C4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C5" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="C5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C7">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C10">
-        <v>2401</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C11">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C12">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C13">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C14">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C15">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C16">
-        <v>80</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C17">
-        <v>443</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>239</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C18">
-        <v>500</v>
+        <v>993</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C19">
-        <v>4500</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C20">
-        <v>143</v>
+        <v>646</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C21">
-        <v>993</v>
+        <v>646</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C22">
-        <v>389</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C23">
-        <v>646</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C24">
-        <v>646</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>244</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C26">
-        <v>1433</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>246</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C27">
-        <v>138</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C28">
-        <v>137</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C29">
-        <v>139</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C30">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C31">
-        <v>2049</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C32">
-        <v>2049</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C33">
-        <v>123</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C34">
-        <v>110</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C35">
-        <v>1813</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>232</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C36">
-        <v>1812</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>250</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C37">
-        <v>3389</v>
+        <v>587</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C38">
-        <v>445</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>214</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>444</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>251</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C40">
-        <v>587</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>252</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C41">
-        <v>465</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C42">
-        <v>444</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>248</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="C43">
-        <v>1434</v>
+        <v>514</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>249</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C44">
-        <v>1525</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>231</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C46">
-        <v>514</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>215</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C47">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
-      </c>
-      <c r="C48">
-        <v>65</v>
+        <v>158</v>
+      </c>
+      <c r="C48" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>180</v>
-      </c>
-      <c r="C49">
-        <v>23</v>
+        <v>157</v>
+      </c>
+      <c r="C49" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
-      </c>
-      <c r="C50">
-        <v>69</v>
+        <v>159</v>
+      </c>
+      <c r="C50" s="24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C66">
-    <sortCondition ref="A7:A66"/>
+  <sheetProtection sort="0" autoFilter="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C63">
+    <sortCondition ref="A4:A63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3380,7 +2975,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3399,19 +2994,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>198</v>
+        <v>97</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3425,7 +3020,7 @@
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="18" t="s">
-        <v>200</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3439,21 +3034,21 @@
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="18" t="s">
-        <v>201</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19"/>
       <c r="B4" s="20" t="s">
-        <v>257</v>
+        <v>155</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="20" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DlukzEIm9eGAbB/egZk4+FltL7m1oi2jFmuvMxmjZFFpvBqSQxu7AUuBydMuQ2sD9sjsmkDZu+UySBW9vqyTQg==" saltValue="nk30D19l22prLeJnA4qXlA==" spinCount="100000" sheet="1" objects="1" scenarios="1" sort="0" autoFilter="0"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3470,10 +3065,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3509,7 +3104,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3517,12 +3112,12 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3554,37 +3149,32 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>18</v>
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A27">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B27" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PCugRULIkoJFfOFVo//wMwEXv3pQvwEGLyLWhWDhedoiHtH24X8PSZrS2oCqC+32lmNoDHyxrT+D/0k4PdY7Ow==" saltValue="HLjKgnGaRnKSBF1AGjxcvA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -3607,98 +3197,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>77</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>102</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>80</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>105</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test XLS file
</commit_message>
<xml_diff>
--- a/fw_rules_test.xlsx
+++ b/fw_rules_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD0BF4-C99C-48E4-9BDB-2DC8EE3A9B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF553B22-A0CE-4C67-8FCA-3D0B7E19C508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="216">
   <si>
     <t>Source Network</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>DMZ1 - semi-trusted - LB services - private addresses</t>
+  </si>
+  <si>
+    <t>split line to multiple line to-zone, from zone</t>
+  </si>
+  <si>
+    <t>set groups tafehub-fw-policy</t>
   </si>
 </sst>
 </file>
@@ -739,7 +745,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,12 +774,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -913,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -956,8 +956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1548,7 +1547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2415,7 +2414,7 @@
       <c r="C1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2426,7 +2425,7 @@
       <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>999</v>
       </c>
     </row>
@@ -2437,7 +2436,7 @@
       <c r="B3" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>0</v>
       </c>
     </row>
@@ -2932,7 +2931,7 @@
       <c r="B48" t="s">
         <v>158</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C48" s="23">
         <v>0</v>
       </c>
     </row>
@@ -2943,7 +2942,7 @@
       <c r="B49" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <v>0</v>
       </c>
     </row>
@@ -2954,7 +2953,7 @@
       <c r="B50" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="23">
         <v>0</v>
       </c>
     </row>
@@ -3183,10 +3182,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AF5221-51D1-4864-A25A-0E399DB24E81}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3199,7 +3198,7 @@
       <c r="A1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3208,30 +3207,30 @@
         <v>78</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" t="s">
-        <v>103</v>
+      <c r="B3" s="21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" t="s">
-        <v>103</v>
+      <c r="B4" s="21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3239,7 +3238,7 @@
       <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3247,7 +3246,7 @@
       <c r="A7" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3255,7 +3254,7 @@
       <c r="A8" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3263,7 +3262,7 @@
       <c r="A9" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3279,7 +3278,12 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3288,7 +3292,17 @@
         <v>105</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>